<commit_message>
update company component structure adding 'email' field and remove 'general service' contacts from staff list
</commit_message>
<xml_diff>
--- a/data/development/userData/contacts.xlsx
+++ b/data/development/userData/contacts.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE07105-36C1-4BCE-8B9A-1185619294CA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CBB6BB-4F9D-49CE-998C-80F7C14B77BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="companies" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,7 +91,107 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Gentry Hardware General Service</t>
+    <t>Johnson Wu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>altecqc@msn.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+86 139 2490 6281</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>David Tsai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>david.tsai@gentry-way.com.tw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+886 (0)955 350 659</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cathy.liu@gentry-way.com.tw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>candy.wu@gentry-way.com.tw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cathy Liu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Candy Wu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>China</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Taiwan R.O.C.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>taiwan.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>china.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISO 9001:2015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iso-9001-2015.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ISO 13485:2016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iso-13485-2016.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ce.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>certifications</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>latitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>longitude</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -99,103 +199,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Johnson Wu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>altecqc@msn.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+86 139 2490 6281</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gentry Way General Service</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>gentry88@ms46.hinet.net</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>David Tsai</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>david.tsai@gentry-way.com.tw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+886 (0)955 350 659</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cathy.liu@gentry-way.com.tw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>candy.wu@gentry-way.com.tw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cathy Liu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Candy Wu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>China</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Taiwan R.O.C.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>taiwan.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>china.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>flag</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>logo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISO 9001:2015</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>iso-9001-2015.jpg</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ISO 13485:2016</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>iso-13485-2016.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ce.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>certifications</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -522,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -533,10 +537,12 @@
     <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="80.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -547,44 +553,71 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2">
+        <v>22.627572000000001</v>
+      </c>
+      <c r="E2">
+        <v>113.32820100000001</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3">
+        <v>23.306155</v>
+      </c>
+      <c r="E3">
+        <v>120.273286</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -613,31 +646,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -648,10 +681,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55866938-584E-4DA7-B8AC-4F0E0C1D5365}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -681,10 +714,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -692,13 +728,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -706,46 +739,24 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -773,23 +784,23 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -802,7 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80811836-4A5A-4B8D-BAA5-6C8BF3AB1CEB}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -817,7 +828,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -825,7 +836,7 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -833,7 +844,7 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -841,7 +852,7 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -849,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>